<commit_message>
no code templates updated for chatgpt ner
</commit_message>
<xml_diff>
--- a/dialbb/no_code/templates/en/scenario.xlsx
+++ b/dialbb/no_code/templates/en/scenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\dialbb\no_code\templates\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E462CF35-A1EB-4F13-B3FE-F0477F6B4DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE6A2EB-72CE-4916-8CF5-F3944ED79F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -124,10 +124,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>#NE_PERSON!=""</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>{$"Generate a sentence to say it's time to end the talk by continuing the conversation in 50 words"}. See you again.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -144,7 +140,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Thank you {#NE_PERSON}! Let me ask you about sandwich. Do you have sandwiches very often?</t>
+    <t>#NE_person!=""</t>
+  </si>
+  <si>
+    <t>Thank you {#NE_person}! Let me ask you about sandwich. Do you have sandwiches very often?</t>
   </si>
 </sst>
 </file>
@@ -574,23 +573,23 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.59765625" style="4"/>
+    <col min="1" max="1" width="8.5703125" style="4"/>
     <col min="2" max="2" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.46484375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.46484375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.59765625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="40.265625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="46.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.59765625" style="4"/>
+    <col min="3" max="3" width="36.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="30">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -616,7 +615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="28.5">
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
@@ -627,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>14</v>
@@ -641,7 +640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="42.75">
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="45">
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
@@ -655,7 +654,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="42.75">
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="45">
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
@@ -669,12 +668,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="42.75">
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="45">
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>2</v>
@@ -686,12 +685,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="28.5">
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>19</v>
@@ -705,20 +704,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="42.75">
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="60">
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" ht="42.75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="60">
       <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1">

</xml_diff>